<commit_message>
Fix bug Rental Item, Inventory
</commit_message>
<xml_diff>
--- a/docs/ItemList.xlsx
+++ b/docs/ItemList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoSoNganh\LapTrinhTrucQuan\IT008_Keytime\it008-keytime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoSoNganh\LapTrinhTrucQuan\IT008_Keytime\it008-keytime\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B8BF6-E902-48A1-BEF1-D4945461ACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBAD454-72D7-4DFE-B0A4-CF8E0891CC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{46725F0B-529E-4380-8339-502F7938FDA4}"/>
   </bookViews>
@@ -36,180 +36,186 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROOM </t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATUS </t>
-  </si>
-  <si>
     <t>NOTE</t>
   </si>
   <si>
-    <t>Dynamic_Clock</t>
-  </si>
-  <si>
-    <t>Relaxing_Sofa</t>
-  </si>
-  <si>
-    <t>Modern_Desk</t>
-  </si>
-  <si>
-    <t>Cozy_Chair</t>
-  </si>
-  <si>
-    <t>Productive_Laptop</t>
-  </si>
-  <si>
-    <t>Indoor_Plant</t>
-  </si>
-  <si>
-    <t>Smart_TV</t>
-  </si>
-  <si>
-    <t>Coffee Table</t>
-  </si>
-  <si>
-    <t>Bluetooth_Speaker</t>
-  </si>
-  <si>
-    <t>Whiteboard</t>
-  </si>
-  <si>
-    <t>Leather Sofa</t>
-  </si>
-  <si>
-    <t>Fitness_Mat</t>
-  </si>
-  <si>
-    <t>Organizer_Drawers</t>
-  </si>
-  <si>
-    <t>Desk_Organizer</t>
-  </si>
-  <si>
-    <t>Standing_Lamp</t>
-  </si>
-  <si>
-    <t>Cozy Blanket</t>
-  </si>
-  <si>
-    <t>Dining_Chairs</t>
-  </si>
-  <si>
-    <t>Wall_Art</t>
-  </si>
-  <si>
-    <t>Smart_Watch</t>
-  </si>
-  <si>
-    <t>Bookshelf</t>
-  </si>
-  <si>
-    <t>Adjustable_Desk</t>
-  </si>
-  <si>
-    <t>Decorative_Plates</t>
-  </si>
-  <si>
-    <t>Yoga_Mat</t>
-  </si>
-  <si>
-    <t>Wall_Mirror</t>
-  </si>
-  <si>
-    <t>Gaming_Chair</t>
-  </si>
-  <si>
-    <t>Stylish clock for your wall.</t>
-  </si>
-  <si>
-    <t>Perfect for a cozy evening.</t>
-  </si>
-  <si>
-    <t>Sleek and modern desk for your office.</t>
-  </si>
-  <si>
-    <t>Comfortable chair for relaxation.</t>
-  </si>
-  <si>
-    <t>A high-performance laptop for work.</t>
-  </si>
-  <si>
-    <t>Bring a touch of nature to your space.</t>
-  </si>
-  <si>
-    <t>Enjoy your favorite shows in high-res.</t>
-  </si>
-  <si>
-    <t>Minimalist coffee table design.</t>
-  </si>
-  <si>
-    <t>Portable speaker for music lovers.</t>
-  </si>
-  <si>
-    <t>Ideal for brainstorming and planning.</t>
-  </si>
-  <si>
-    <t>Luxurious sofa for a touch of class.</t>
-  </si>
-  <si>
-    <t>Stay active with a comfortable mat.</t>
-  </si>
-  <si>
-    <t>Keep your space tidy and organized.</t>
-  </si>
-  <si>
-    <t>Keep your desk essentials in order.</t>
-  </si>
-  <si>
-    <t>Adjustable lamp for focused lighting.</t>
-  </si>
-  <si>
-    <t>Soft blanket for chilly evenings.</t>
-  </si>
-  <si>
-    <t>Elegant chairs for your dining area.</t>
-  </si>
-  <si>
-    <t>Decorate your walls with unique art.</t>
-  </si>
-  <si>
-    <t>Stay connected with a smartwatch.</t>
-  </si>
-  <si>
-    <t>Display your favorite books and more.</t>
-  </si>
-  <si>
-    <t>Perfect for your yoga and exercise.</t>
-  </si>
-  <si>
-    <t>Add depth and style to your room.</t>
-  </si>
-  <si>
-    <t>Comfortable chair for gaming sessions.</t>
-  </si>
-  <si>
-    <t>Customize your workspace with this desk.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Beautiful plates for your dining table.</t>
-  </si>
-  <si>
-    <t>IDLE</t>
-  </si>
-  <si>
     <t>Great for unwinding.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME           </t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPTION                       </t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>Comfortable_Bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideal for a good night's sleep.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDLE  </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relaxing_Sofa  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfect for a cozy evening.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study_Desk     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suitable for focused work.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee_Table   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great for coffee breaks.          </t>
+  </si>
+  <si>
+    <t>Needs repair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading_Chair  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comfortable for reading.          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitchen_Table  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space for meals and discussions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desk_Lamp      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides focused lighting.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean_Bag_Chair </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relaxed seating option.           </t>
+  </si>
+  <si>
+    <t>Conference_Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For meetings and collaborations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standing_Desk  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotes an active work style.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printer        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For printing documents.           </t>
+  </si>
+  <si>
+    <t>Needs maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whiteboard     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideal for brainstorming.          </t>
+  </si>
+  <si>
+    <t>Desktop_Computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-performance workstation.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recliner       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfect for a quick nap.          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office_Plant   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brings a touch of nature.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Cooler   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keeps everyone hydrated.          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coat_Rack      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizes coats and jackets.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filing_Cabinet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For organizing important files.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desk_Chair     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ergonomic seating option.         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projector      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For presentations and meetings.   </t>
+  </si>
+  <si>
+    <t>Needs replacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wall_Clock     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keeps track of time.              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean_Bag       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casual and comfortable seating.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standing_Fan   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides additional ventilation.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desk_Organizer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keeps desk essentials in order.   </t>
   </si>
 </sst>
 </file>
@@ -581,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B620AD6B-1ECD-4E14-8E61-82FD0EB1EC3A}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -601,19 +607,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -621,16 +627,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -638,19 +647,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>456</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -658,16 +667,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>789</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -675,16 +687,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>234</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -692,16 +707,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>567</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -709,16 +727,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>890</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -726,16 +747,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>345</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -743,16 +767,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>678</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -760,16 +787,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C10">
-        <v>901</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -777,16 +807,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C11">
-        <v>432</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -794,16 +827,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>765</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -811,16 +847,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C13">
-        <v>876</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -828,16 +867,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>543</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -845,16 +887,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C15">
-        <v>678</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -862,186 +907,199 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C16">
-        <v>987</v>
+        <v>115</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>345</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>654</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>321</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C20">
-        <v>876</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C21">
-        <v>543</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
         <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C22">
-        <v>234</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C23">
-        <v>567</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C24">
-        <v>890</v>
+        <v>123</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C25">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>222</v>
-      </c>
-      <c r="D26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>